<commit_message>
remove characterhelper, refactor mode
</commit_message>
<xml_diff>
--- a/tests/game/wow/wlk/dataset/test_dataset.xlsx
+++ b/tests/game/wow/wlk/dataset/test_dataset.xlsx
@@ -9,7 +9,7 @@
     <sheet state="visible" name="build" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="build_group" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="client" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="target_leader" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="target_key_mapping" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="mode" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Talent" sheetId="9" r:id="rId12"/>
   </sheets>
@@ -128,7 +128,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">这个表记录了在不同的 setup 下, 为了选中位于谋个 label 窗口内的角色, 应该按下什么快捷键 (宏命令).
+        <t xml:space="preserve">这个表记录了在不同的 setup 下, 为了选中位于某个 label 窗口内的角色, 应该按下什么快捷键 (宏命令).
 	-Sanhe Hu</t>
       </text>
     </comment>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="295">
   <si>
     <r>
       <rPr/>
@@ -291,6 +291,27 @@
     <t>window</t>
   </si>
   <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>is_leader_1</t>
+  </si>
+  <si>
+    <t>is_leader_2</t>
+  </si>
+  <si>
+    <t>is_tank_1</t>
+  </si>
+  <si>
+    <t>is_tank_2</t>
+  </si>
+  <si>
+    <t>is_dr_pala_1</t>
+  </si>
+  <si>
+    <t>is_dr_pala_2</t>
+  </si>
+  <si>
     <t>r_1_to_5</t>
   </si>
   <si>
@@ -456,7 +477,7 @@
     <t>zhTW_1176_664</t>
   </si>
   <si>
-    <t>setup</t>
+    <t>mapping</t>
   </si>
   <si>
     <t>keyboard</t>
@@ -474,61 +495,10 @@
     <t>mode</t>
   </si>
   <si>
-    <t>active_chars_include1</t>
-  </si>
-  <si>
-    <t>active_chars_include2</t>
-  </si>
-  <si>
-    <t>active_chars_include3</t>
-  </si>
-  <si>
-    <t>active_chars_exclude1</t>
-  </si>
-  <si>
-    <t>active_chars_exclude2</t>
-  </si>
-  <si>
-    <t>active_chars_exclude3</t>
-  </si>
-  <si>
-    <t>login_chars_include1</t>
-  </si>
-  <si>
-    <t>login_chars_include2</t>
-  </si>
-  <si>
-    <t>login_chars_include3</t>
-  </si>
-  <si>
-    <t>login_chars_exclude1</t>
-  </si>
-  <si>
-    <t>login_chars_exclude2</t>
-  </si>
-  <si>
-    <t>login_chars_exclude3</t>
-  </si>
-  <si>
-    <t>target_leader</t>
-  </si>
-  <si>
-    <t>leader1</t>
-  </si>
-  <si>
-    <t>leader2</t>
-  </si>
-  <si>
-    <t>tank1</t>
-  </si>
-  <si>
-    <t>tank2</t>
-  </si>
-  <si>
-    <t>dr_pala1</t>
-  </si>
-  <si>
-    <t>dr_pala2</t>
+    <t>chars</t>
+  </si>
+  <si>
+    <t>target_key_mapping</t>
   </si>
   <si>
     <t>alliance_r_abcde_solo_dungeon</t>
@@ -1131,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1162,13 +1132,10 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1238,7 +1205,7 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="target_leader-style">
+    <tableStyle count="3" pivot="0" name="target_key_mapping-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -1328,11 +1295,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C190" displayName="Table_4" name="Table_4" id="4">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J190" displayName="Table_4" name="Table_4" id="4">
+  <tableColumns count="10">
     <tableColumn name="build_group" id="1"/>
     <tableColumn name="build" id="2"/>
     <tableColumn name="window" id="3"/>
+    <tableColumn name="is_active" id="4"/>
+    <tableColumn name="is_leader_1" id="5"/>
+    <tableColumn name="is_leader_2" id="6"/>
+    <tableColumn name="is_tank_1" id="7"/>
+    <tableColumn name="is_tank_2" id="8"/>
+    <tableColumn name="is_dr_pala_1" id="9"/>
+    <tableColumn name="is_dr_pala_2" id="10"/>
   </tableColumns>
   <tableStyleInfo name="build_group-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -1399,38 +1373,21 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C10" displayName="Table_6" name="Table_6" id="6">
   <tableColumns count="3">
-    <tableColumn name="setup" id="1"/>
+    <tableColumn name="mapping" id="1"/>
     <tableColumn name="window" id="2"/>
     <tableColumn name="keyboard" id="3"/>
   </tableColumns>
-  <tableStyleInfo name="target_leader-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="target_key_mapping-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:U10" displayName="Table_7" name="Table_7" id="7">
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D10" displayName="Table_7" name="Table_7" id="7">
+  <tableColumns count="4">
     <tableColumn name="mode" id="1"/>
     <tableColumn name="client" id="2"/>
-    <tableColumn name="active_chars_include1" id="3"/>
-    <tableColumn name="active_chars_include2" id="4"/>
-    <tableColumn name="active_chars_include3" id="5"/>
-    <tableColumn name="active_chars_exclude1" id="6"/>
-    <tableColumn name="active_chars_exclude2" id="7"/>
-    <tableColumn name="active_chars_exclude3" id="8"/>
-    <tableColumn name="login_chars_include1" id="9"/>
-    <tableColumn name="login_chars_include2" id="10"/>
-    <tableColumn name="login_chars_include3" id="11"/>
-    <tableColumn name="login_chars_exclude1" id="12"/>
-    <tableColumn name="login_chars_exclude2" id="13"/>
-    <tableColumn name="login_chars_exclude3" id="14"/>
-    <tableColumn name="target_leader" id="15"/>
-    <tableColumn name="leader1" id="16"/>
-    <tableColumn name="leader2" id="17"/>
-    <tableColumn name="tank1" id="18"/>
-    <tableColumn name="tank2" id="19"/>
-    <tableColumn name="dr_pala1" id="20"/>
-    <tableColumn name="dr_pala2" id="21"/>
+    <tableColumn name="chars" id="3"/>
+    <tableColumn name="target_key_mapping" id="4"/>
   </tableColumns>
   <tableStyleInfo name="mode-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -4268,8 +4225,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="37.63"/>
-    <col customWidth="1" min="3" max="3" width="18.38"/>
+    <col customWidth="1" min="1" max="1" width="17.75"/>
+    <col customWidth="1" min="2" max="2" width="27.13"/>
+    <col customWidth="1" min="3" max="3" width="7.13"/>
+    <col customWidth="1" min="4" max="4" width="8.0"/>
+    <col customWidth="1" min="5" max="6" width="10.13"/>
+    <col customWidth="1" min="7" max="8" width="8.63"/>
+    <col customWidth="1" min="9" max="10" width="11.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4282,1101 +4244,2525 @@
       <c r="C1" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
+      <c r="D2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3">
         <v>3.0</v>
       </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3">
         <v>4.0</v>
       </c>
+      <c r="D5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3">
         <v>5.0</v>
       </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3">
         <v>1.0</v>
       </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C8" s="3">
         <v>2.0</v>
       </c>
+      <c r="D8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C9" s="3">
         <v>3.0</v>
       </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C10" s="3">
         <v>4.0</v>
       </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3">
         <v>5.0</v>
       </c>
+      <c r="D11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C12" s="3">
         <v>6.0</v>
       </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C13" s="3">
         <v>7.0</v>
       </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C14" s="3">
         <v>8.0</v>
       </c>
+      <c r="D14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C15" s="3">
         <v>9.0</v>
       </c>
+      <c r="D15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3">
         <v>10.0</v>
       </c>
+      <c r="D16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3">
         <v>1.0</v>
       </c>
+      <c r="D17" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3">
         <v>2.0</v>
       </c>
+      <c r="D18" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3">
         <v>3.0</v>
       </c>
+      <c r="D19" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C20" s="3">
         <v>4.0</v>
       </c>
+      <c r="D20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C21" s="3">
         <v>5.0</v>
       </c>
+      <c r="D21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C22" s="3">
         <v>1.0</v>
       </c>
+      <c r="D22" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C23" s="3">
         <v>2.0</v>
       </c>
+      <c r="D23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C24" s="3">
         <v>3.0</v>
       </c>
+      <c r="D24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C25" s="3">
         <v>4.0</v>
       </c>
+      <c r="D25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C26" s="3">
         <v>5.0</v>
       </c>
+      <c r="D26" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
     </row>
     <row r="29">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
     </row>
     <row r="30">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
     </row>
     <row r="31">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
     </row>
     <row r="32">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
     </row>
     <row r="33">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
     </row>
     <row r="35">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
     </row>
     <row r="37">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
     <row r="39">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
     <row r="40">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
     </row>
     <row r="41">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
     </row>
     <row r="42">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
     </row>
     <row r="43">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
     </row>
     <row r="44">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
     </row>
     <row r="45">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
     </row>
     <row r="46">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
     </row>
     <row r="47">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
     </row>
     <row r="48">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
     </row>
     <row r="49">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
     </row>
     <row r="50">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
     </row>
     <row r="51">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
     </row>
     <row r="52">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
     </row>
     <row r="53">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
     </row>
     <row r="54">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
     </row>
     <row r="55">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
     </row>
     <row r="56">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
     </row>
     <row r="57">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
     </row>
     <row r="58">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
     </row>
     <row r="59">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
     </row>
     <row r="60">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
     </row>
     <row r="61">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
     </row>
     <row r="62">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
     </row>
     <row r="63">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
     </row>
     <row r="64">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
     </row>
     <row r="65">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
     </row>
     <row r="66">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
     </row>
     <row r="67">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
     </row>
     <row r="68">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
     </row>
     <row r="69">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
     </row>
     <row r="70">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
     </row>
     <row r="71">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
     </row>
     <row r="72">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
     </row>
     <row r="73">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
     </row>
     <row r="74">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
     </row>
     <row r="75">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
     </row>
     <row r="76">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
     </row>
     <row r="77">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
     </row>
     <row r="78">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
     </row>
     <row r="79">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
     </row>
     <row r="80">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
     </row>
     <row r="81">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
     </row>
     <row r="82">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
     </row>
     <row r="83">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
     </row>
     <row r="84">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
     </row>
     <row r="85">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
     </row>
     <row r="86">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
     </row>
     <row r="87">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
     </row>
     <row r="88">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
     </row>
     <row r="89">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
     </row>
     <row r="90">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
     </row>
     <row r="91">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
     </row>
     <row r="92">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
     </row>
     <row r="93">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
     </row>
     <row r="94">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
     </row>
     <row r="95">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
     </row>
     <row r="96">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
     </row>
     <row r="97">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
     </row>
     <row r="98">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
     </row>
     <row r="99">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
     </row>
     <row r="100">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="4"/>
     </row>
     <row r="101">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
+      <c r="J101" s="4"/>
     </row>
     <row r="102">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
     </row>
     <row r="103">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+      <c r="J103" s="4"/>
     </row>
     <row r="104">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+      <c r="J104" s="4"/>
     </row>
     <row r="105">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="J105" s="4"/>
     </row>
     <row r="106">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="4"/>
     </row>
     <row r="107">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="J107" s="4"/>
     </row>
     <row r="108">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
     </row>
     <row r="109">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="4"/>
     </row>
     <row r="110">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="4"/>
     </row>
     <row r="111">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
     </row>
     <row r="112">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
     </row>
     <row r="113">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4"/>
     </row>
     <row r="114">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4"/>
     </row>
     <row r="115">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4"/>
     </row>
     <row r="116">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+      <c r="J116" s="4"/>
     </row>
     <row r="117">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+      <c r="J117" s="4"/>
     </row>
     <row r="118">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="4"/>
     </row>
     <row r="119">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4"/>
     </row>
     <row r="120">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="4"/>
     </row>
     <row r="121">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="4"/>
+      <c r="J121" s="4"/>
     </row>
     <row r="122">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+      <c r="J122" s="4"/>
     </row>
     <row r="123">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="4"/>
+      <c r="J123" s="4"/>
     </row>
     <row r="124">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+      <c r="J124" s="4"/>
     </row>
     <row r="125">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
     </row>
     <row r="126">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4"/>
     </row>
     <row r="127">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="4"/>
+      <c r="J127" s="4"/>
     </row>
     <row r="128">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+      <c r="J128" s="4"/>
     </row>
     <row r="129">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="4"/>
+      <c r="J129" s="4"/>
     </row>
     <row r="130">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="4"/>
+      <c r="J130" s="4"/>
     </row>
     <row r="131">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="4"/>
+      <c r="J131" s="4"/>
     </row>
     <row r="132">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="4"/>
     </row>
     <row r="133">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4"/>
     </row>
     <row r="134">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
     </row>
     <row r="135">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4"/>
     </row>
     <row r="136">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+      <c r="J136" s="4"/>
     </row>
     <row r="137">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+      <c r="J137" s="4"/>
     </row>
     <row r="138">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
+      <c r="J138" s="4"/>
     </row>
     <row r="139">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+      <c r="J139" s="4"/>
     </row>
     <row r="140">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4"/>
     </row>
     <row r="141">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+      <c r="J141" s="4"/>
     </row>
     <row r="142">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="4"/>
+      <c r="J142" s="4"/>
     </row>
     <row r="143">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+      <c r="J143" s="4"/>
     </row>
     <row r="144">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="4"/>
+      <c r="J144" s="4"/>
     </row>
     <row r="145">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="4"/>
+      <c r="J145" s="4"/>
     </row>
     <row r="146">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="4"/>
     </row>
     <row r="147">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
     </row>
     <row r="148">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="4"/>
+      <c r="J148" s="4"/>
     </row>
     <row r="149">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+      <c r="H149" s="4"/>
+      <c r="I149" s="4"/>
+      <c r="J149" s="4"/>
     </row>
     <row r="150">
       <c r="A150" s="4"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
+      <c r="H150" s="4"/>
+      <c r="I150" s="4"/>
+      <c r="J150" s="4"/>
     </row>
     <row r="151">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+      <c r="H151" s="4"/>
+      <c r="I151" s="4"/>
+      <c r="J151" s="4"/>
     </row>
     <row r="152">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="4"/>
+      <c r="I152" s="4"/>
+      <c r="J152" s="4"/>
     </row>
     <row r="153">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
+      <c r="H153" s="4"/>
+      <c r="I153" s="4"/>
+      <c r="J153" s="4"/>
     </row>
     <row r="154">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="4"/>
+      <c r="J154" s="4"/>
     </row>
     <row r="155">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
+      <c r="H155" s="4"/>
+      <c r="I155" s="4"/>
+      <c r="J155" s="4"/>
     </row>
     <row r="156">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+      <c r="H156" s="4"/>
+      <c r="I156" s="4"/>
+      <c r="J156" s="4"/>
     </row>
     <row r="157">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="4"/>
+      <c r="H157" s="4"/>
+      <c r="I157" s="4"/>
+      <c r="J157" s="4"/>
     </row>
     <row r="158">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="4"/>
+      <c r="H158" s="4"/>
+      <c r="I158" s="4"/>
+      <c r="J158" s="4"/>
     </row>
     <row r="159">
       <c r="A159" s="4"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="4"/>
+      <c r="H159" s="4"/>
+      <c r="I159" s="4"/>
+      <c r="J159" s="4"/>
     </row>
     <row r="160">
       <c r="A160" s="4"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
+      <c r="H160" s="4"/>
+      <c r="I160" s="4"/>
+      <c r="J160" s="4"/>
     </row>
     <row r="161">
       <c r="A161" s="4"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
+      <c r="H161" s="4"/>
+      <c r="I161" s="4"/>
+      <c r="J161" s="4"/>
     </row>
     <row r="162">
       <c r="A162" s="4"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
+      <c r="H162" s="4"/>
+      <c r="I162" s="4"/>
+      <c r="J162" s="4"/>
     </row>
     <row r="163">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+      <c r="H163" s="4"/>
+      <c r="I163" s="4"/>
+      <c r="J163" s="4"/>
     </row>
     <row r="164">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="4"/>
+      <c r="I164" s="4"/>
+      <c r="J164" s="4"/>
     </row>
     <row r="165">
       <c r="A165" s="4"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
+      <c r="H165" s="4"/>
+      <c r="I165" s="4"/>
+      <c r="J165" s="4"/>
     </row>
     <row r="166">
       <c r="A166" s="4"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="4"/>
+      <c r="I166" s="4"/>
+      <c r="J166" s="4"/>
     </row>
     <row r="167">
       <c r="A167" s="4"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
+      <c r="H167" s="4"/>
+      <c r="I167" s="4"/>
+      <c r="J167" s="4"/>
     </row>
     <row r="168">
       <c r="A168" s="4"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
+      <c r="D168" s="4"/>
+      <c r="E168" s="4"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
+      <c r="H168" s="4"/>
+      <c r="I168" s="4"/>
+      <c r="J168" s="4"/>
     </row>
     <row r="169">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
+      <c r="D169" s="4"/>
+      <c r="E169" s="4"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
+      <c r="H169" s="4"/>
+      <c r="I169" s="4"/>
+      <c r="J169" s="4"/>
     </row>
     <row r="170">
       <c r="A170" s="4"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="4"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="4"/>
+      <c r="H170" s="4"/>
+      <c r="I170" s="4"/>
+      <c r="J170" s="4"/>
     </row>
     <row r="171">
       <c r="A171" s="4"/>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
+      <c r="H171" s="4"/>
+      <c r="I171" s="4"/>
+      <c r="J171" s="4"/>
     </row>
     <row r="172">
       <c r="A172" s="4"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+      <c r="J172" s="4"/>
     </row>
     <row r="173">
       <c r="A173" s="4"/>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
+      <c r="H173" s="4"/>
+      <c r="I173" s="4"/>
+      <c r="J173" s="4"/>
     </row>
     <row r="174">
       <c r="A174" s="4"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="4"/>
+      <c r="H174" s="4"/>
+      <c r="I174" s="4"/>
+      <c r="J174" s="4"/>
     </row>
     <row r="175">
       <c r="A175" s="4"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="4"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="4"/>
+      <c r="H175" s="4"/>
+      <c r="I175" s="4"/>
+      <c r="J175" s="4"/>
     </row>
     <row r="176">
       <c r="A176" s="4"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+      <c r="J176" s="4"/>
     </row>
     <row r="177">
       <c r="A177" s="4"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
     </row>
     <row r="178">
       <c r="A178" s="4"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+      <c r="J178" s="4"/>
     </row>
     <row r="179">
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
+      <c r="D179" s="4"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
+      <c r="H179" s="4"/>
+      <c r="I179" s="4"/>
+      <c r="J179" s="4"/>
     </row>
     <row r="180">
       <c r="A180" s="4"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
+      <c r="H180" s="4"/>
+      <c r="I180" s="4"/>
+      <c r="J180" s="4"/>
     </row>
     <row r="181">
       <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="4"/>
+      <c r="H181" s="4"/>
+      <c r="I181" s="4"/>
+      <c r="J181" s="4"/>
     </row>
     <row r="182">
       <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
+      <c r="D182" s="4"/>
+      <c r="E182" s="4"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="4"/>
+      <c r="H182" s="4"/>
+      <c r="I182" s="4"/>
+      <c r="J182" s="4"/>
     </row>
     <row r="183">
       <c r="A183" s="4"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
+      <c r="D183" s="4"/>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
+      <c r="H183" s="4"/>
+      <c r="I183" s="4"/>
+      <c r="J183" s="4"/>
     </row>
     <row r="184">
       <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="4"/>
+      <c r="H184" s="4"/>
+      <c r="I184" s="4"/>
+      <c r="J184" s="4"/>
     </row>
     <row r="185">
       <c r="A185" s="4"/>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="4"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="4"/>
+      <c r="H185" s="4"/>
+      <c r="I185" s="4"/>
+      <c r="J185" s="4"/>
     </row>
     <row r="186">
       <c r="A186" s="4"/>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="4"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="4"/>
+      <c r="H186" s="4"/>
+      <c r="I186" s="4"/>
+      <c r="J186" s="4"/>
     </row>
     <row r="187">
       <c r="A187" s="4"/>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="4"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="4"/>
+      <c r="H187" s="4"/>
+      <c r="I187" s="4"/>
+      <c r="J187" s="4"/>
     </row>
     <row r="188">
       <c r="A188" s="4"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="4"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="4"/>
+      <c r="H188" s="4"/>
+      <c r="I188" s="4"/>
+      <c r="J188" s="4"/>
     </row>
     <row r="189">
       <c r="A189" s="4"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="4"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="4"/>
+      <c r="H189" s="4"/>
+      <c r="I189" s="4"/>
+      <c r="J189" s="4"/>
     </row>
     <row r="190">
       <c r="A190" s="4"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="4"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="4"/>
+      <c r="H190" s="4"/>
+      <c r="I190" s="4"/>
+      <c r="J190" s="4"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -5429,109 +6815,109 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="AH1" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
@@ -5546,13 +6932,13 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -5599,13 +6985,13 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D3" s="4">
         <v>125.0</v>
@@ -5714,13 +7100,13 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -5789,35 +7175,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B2" s="3">
         <v>1.0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B3" s="3">
         <v>10.0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
@@ -5879,376 +7265,122 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.63"/>
-    <col customWidth="1" min="2" max="2" width="15.0"/>
-    <col customWidth="1" min="3" max="5" width="18.75"/>
-    <col customWidth="1" min="6" max="8" width="19.13"/>
-    <col customWidth="1" min="9" max="11" width="18.0"/>
-    <col customWidth="1" min="12" max="15" width="18.38"/>
-    <col customWidth="1" min="16" max="21" width="23.25"/>
+    <col customWidth="1" min="1" max="1" width="34.88"/>
+    <col customWidth="1" min="2" max="2" width="18.63"/>
+    <col customWidth="1" min="3" max="3" width="22.63"/>
+    <col customWidth="1" min="4" max="4" width="17.25"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="M1" s="10" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="B4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P1" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="11"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" s="11"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="U5" s="11"/>
+      <c r="B5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P2:U5">
-      <formula1>build!$A$2:$A$996</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B5">
       <formula1>client!$A$2:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:N5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C5">
       <formula1>build_group!$A$2:$A$989</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O2:O5">
-      <formula1>target_leader!$A$2:$A$10</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D5">
+      <formula1>target_key_mapping!$A$2:$A$10</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId2"/>
@@ -6278,18 +7410,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
@@ -6297,63 +7429,63 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11">
@@ -6361,23 +7493,23 @@
         <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14">
@@ -6385,47 +7517,47 @@
         <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20">
@@ -6433,39 +7565,39 @@
         <v>35</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25">
@@ -6473,47 +7605,47 @@
         <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31">
@@ -6521,7 +7653,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32">
@@ -6529,47 +7661,47 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38">
@@ -6577,7 +7709,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39">
@@ -6585,79 +7717,79 @@
         <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49">
@@ -6665,55 +7797,55 @@
         <v>30</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56">
@@ -6721,673 +7853,673 @@
         <v>34</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3"/>
       <c r="B67" s="3" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3"/>
       <c r="B68" s="3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="7"/>
       <c r="B69" s="3" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="7"/>
       <c r="B70" s="3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="7"/>
       <c r="B71" s="3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="7"/>
       <c r="B72" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="7"/>
       <c r="B73" s="3" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="7"/>
       <c r="B74" s="3" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="7"/>
       <c r="B75" s="3" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="7"/>
       <c r="B76" s="3" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="7"/>
       <c r="B77" s="3" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="7"/>
       <c r="B78" s="3" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="7"/>
       <c r="B79" s="3" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="7"/>
       <c r="B80" s="3" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="7"/>
       <c r="B81" s="3" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="7"/>
       <c r="B82" s="3" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="7"/>
       <c r="B83" s="3" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="7"/>
       <c r="B84" s="3" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="7"/>
       <c r="B85" s="3" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="7"/>
       <c r="B86" s="3" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="7"/>
       <c r="B87" s="3" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="7"/>
       <c r="B88" s="3" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="7"/>
       <c r="B89" s="3" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="7"/>
       <c r="B90" s="3" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="7"/>
       <c r="B91" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="7"/>
       <c r="B92" s="3" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="7"/>
       <c r="B93" s="3" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="7"/>
       <c r="B94" s="3" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="7"/>
       <c r="B95" s="3" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="7"/>
       <c r="B96" s="3" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="7"/>
       <c r="B97" s="3" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="7"/>
       <c r="B98" s="3" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="7"/>
       <c r="B99" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="7"/>
       <c r="B100" s="3" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="7"/>
       <c r="B101" s="3" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="7"/>
       <c r="B102" s="3" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="7"/>
       <c r="B103" s="3" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="7"/>
       <c r="B104" s="3" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="7"/>
       <c r="B105" s="3" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="7"/>
       <c r="B106" s="3" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="7"/>
       <c r="B107" s="3" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="7"/>
       <c r="B108" s="3" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="7"/>
       <c r="B109" s="3" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="7"/>
       <c r="B110" s="3" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="7"/>
       <c r="B111" s="3" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="7"/>
       <c r="B112" s="3" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="7"/>
       <c r="B113" s="3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="7"/>
       <c r="B114" s="3" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="7"/>
       <c r="B115" s="3" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="7"/>
       <c r="B116" s="3" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="7"/>
       <c r="B117" s="3" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="7"/>
       <c r="B118" s="3" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7"/>
       <c r="B119" s="3" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="7"/>
       <c r="B120" s="3" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="7"/>
       <c r="B121" s="3" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="7"/>
       <c r="B122" s="3" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="7"/>
       <c r="B123" s="3" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="7"/>
       <c r="B124" s="3" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="125">
-      <c r="B125" s="12"/>
+      <c r="B125" s="10"/>
     </row>
     <row r="126">
-      <c r="B126" s="12"/>
+      <c r="B126" s="10"/>
     </row>
     <row r="127">
-      <c r="B127" s="12"/>
+      <c r="B127" s="10"/>
     </row>
     <row r="128">
-      <c r="B128" s="12"/>
+      <c r="B128" s="10"/>
     </row>
     <row r="129">
-      <c r="B129" s="12"/>
+      <c r="B129" s="10"/>
     </row>
     <row r="130">
-      <c r="B130" s="12"/>
+      <c r="B130" s="10"/>
     </row>
     <row r="131">
-      <c r="B131" s="12"/>
+      <c r="B131" s="10"/>
     </row>
     <row r="132">
-      <c r="B132" s="12"/>
+      <c r="B132" s="10"/>
     </row>
     <row r="133">
-      <c r="B133" s="12"/>
+      <c r="B133" s="10"/>
     </row>
     <row r="134">
-      <c r="B134" s="12"/>
+      <c r="B134" s="10"/>
     </row>
     <row r="135">
-      <c r="B135" s="12"/>
+      <c r="B135" s="10"/>
     </row>
     <row r="136">
-      <c r="B136" s="12"/>
+      <c r="B136" s="10"/>
     </row>
     <row r="137">
-      <c r="B137" s="12"/>
+      <c r="B137" s="10"/>
     </row>
     <row r="138">
-      <c r="B138" s="12"/>
+      <c r="B138" s="10"/>
     </row>
     <row r="139">
-      <c r="B139" s="12"/>
+      <c r="B139" s="10"/>
     </row>
     <row r="140">
-      <c r="B140" s="12"/>
+      <c r="B140" s="10"/>
     </row>
     <row r="141">
-      <c r="B141" s="12"/>
+      <c r="B141" s="10"/>
     </row>
     <row r="142">
-      <c r="B142" s="12"/>
+      <c r="B142" s="10"/>
     </row>
     <row r="143">
-      <c r="B143" s="12"/>
+      <c r="B143" s="10"/>
     </row>
     <row r="144">
-      <c r="B144" s="12"/>
+      <c r="B144" s="10"/>
     </row>
     <row r="145">
-      <c r="B145" s="12"/>
+      <c r="B145" s="10"/>
     </row>
     <row r="146">
-      <c r="B146" s="12"/>
+      <c r="B146" s="10"/>
     </row>
     <row r="147">
-      <c r="B147" s="12"/>
+      <c r="B147" s="10"/>
     </row>
     <row r="148">
-      <c r="B148" s="12"/>
+      <c r="B148" s="10"/>
     </row>
     <row r="149">
-      <c r="B149" s="12"/>
+      <c r="B149" s="10"/>
     </row>
     <row r="150">
-      <c r="B150" s="12"/>
+      <c r="B150" s="10"/>
     </row>
     <row r="151">
-      <c r="B151" s="12"/>
+      <c r="B151" s="10"/>
     </row>
     <row r="152">
-      <c r="B152" s="12"/>
+      <c r="B152" s="10"/>
     </row>
     <row r="153">
-      <c r="B153" s="12"/>
+      <c r="B153" s="10"/>
     </row>
     <row r="154">
-      <c r="B154" s="12"/>
+      <c r="B154" s="10"/>
     </row>
     <row r="155">
-      <c r="B155" s="12"/>
+      <c r="B155" s="10"/>
     </row>
     <row r="156">
-      <c r="B156" s="12"/>
+      <c r="B156" s="10"/>
     </row>
     <row r="157">
-      <c r="B157" s="12"/>
+      <c r="B157" s="10"/>
     </row>
     <row r="158">
-      <c r="B158" s="12"/>
+      <c r="B158" s="10"/>
     </row>
     <row r="159">
-      <c r="B159" s="12"/>
+      <c r="B159" s="10"/>
     </row>
     <row r="160">
-      <c r="B160" s="12"/>
+      <c r="B160" s="10"/>
     </row>
     <row r="161">
-      <c r="B161" s="12"/>
+      <c r="B161" s="10"/>
     </row>
     <row r="162">
-      <c r="B162" s="12"/>
+      <c r="B162" s="10"/>
     </row>
     <row r="163">
-      <c r="B163" s="12"/>
+      <c r="B163" s="10"/>
     </row>
     <row r="164">
-      <c r="B164" s="12"/>
+      <c r="B164" s="10"/>
     </row>
     <row r="165">
-      <c r="B165" s="12"/>
+      <c r="B165" s="10"/>
     </row>
     <row r="166">
-      <c r="B166" s="12"/>
+      <c r="B166" s="10"/>
     </row>
     <row r="167">
-      <c r="B167" s="12"/>
+      <c r="B167" s="10"/>
     </row>
     <row r="168">
-      <c r="B168" s="12"/>
+      <c r="B168" s="10"/>
     </row>
     <row r="169">
-      <c r="B169" s="12"/>
+      <c r="B169" s="10"/>
     </row>
     <row r="170">
-      <c r="B170" s="12"/>
+      <c r="B170" s="10"/>
     </row>
     <row r="171">
-      <c r="B171" s="12"/>
+      <c r="B171" s="10"/>
     </row>
     <row r="172">
-      <c r="B172" s="12"/>
+      <c r="B172" s="10"/>
     </row>
     <row r="173">
-      <c r="B173" s="12"/>
+      <c r="B173" s="10"/>
     </row>
     <row r="174">
-      <c r="B174" s="12"/>
+      <c r="B174" s="10"/>
     </row>
     <row r="175">
-      <c r="B175" s="12"/>
+      <c r="B175" s="10"/>
     </row>
     <row r="176">
-      <c r="B176" s="12"/>
+      <c r="B176" s="10"/>
     </row>
     <row r="177">
-      <c r="B177" s="12"/>
+      <c r="B177" s="10"/>
     </row>
     <row r="178">
-      <c r="B178" s="12"/>
+      <c r="B178" s="10"/>
     </row>
     <row r="179">
-      <c r="B179" s="12"/>
+      <c r="B179" s="10"/>
     </row>
     <row r="180">
-      <c r="B180" s="12"/>
+      <c r="B180" s="10"/>
     </row>
     <row r="181">
-      <c r="B181" s="12"/>
+      <c r="B181" s="10"/>
     </row>
     <row r="182">
-      <c r="B182" s="12"/>
+      <c r="B182" s="10"/>
     </row>
     <row r="183">
-      <c r="B183" s="12"/>
+      <c r="B183" s="10"/>
     </row>
     <row r="184">
-      <c r="B184" s="12"/>
+      <c r="B184" s="10"/>
     </row>
     <row r="185">
-      <c r="B185" s="12"/>
+      <c r="B185" s="10"/>
     </row>
     <row r="186">
-      <c r="B186" s="12"/>
+      <c r="B186" s="10"/>
     </row>
     <row r="187">
-      <c r="B187" s="12"/>
+      <c r="B187" s="10"/>
     </row>
     <row r="188">
-      <c r="B188" s="12"/>
+      <c r="B188" s="10"/>
     </row>
     <row r="189">
-      <c r="B189" s="12"/>
+      <c r="B189" s="10"/>
     </row>
     <row r="190">
-      <c r="B190" s="12"/>
+      <c r="B190" s="10"/>
     </row>
     <row r="191">
-      <c r="B191" s="12"/>
+      <c r="B191" s="10"/>
     </row>
     <row r="192">
       <c r="A192" s="11"/>
-      <c r="B192" s="12"/>
+      <c r="B192" s="10"/>
     </row>
     <row r="193">
       <c r="A193" s="11"/>
-      <c r="B193" s="12"/>
+      <c r="B193" s="10"/>
     </row>
     <row r="194">
       <c r="A194" s="11"/>
-      <c r="B194" s="12"/>
+      <c r="B194" s="10"/>
     </row>
     <row r="195">
       <c r="A195" s="11"/>
-      <c r="B195" s="12"/>
+      <c r="B195" s="10"/>
     </row>
     <row r="196">
       <c r="A196" s="11"/>
-      <c r="B196" s="12"/>
+      <c r="B196" s="10"/>
     </row>
     <row r="197">
       <c r="A197" s="11"/>
-      <c r="B197" s="12"/>
+      <c r="B197" s="10"/>
     </row>
     <row r="198">
       <c r="A198" s="11"/>
-      <c r="B198" s="12"/>
+      <c r="B198" s="10"/>
     </row>
     <row r="199">
       <c r="A199" s="11"/>
-      <c r="B199" s="12"/>
+      <c r="B199" s="10"/>
     </row>
     <row r="200">
       <c r="A200" s="11"/>
-      <c r="B200" s="12"/>
+      <c r="B200" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>